<commit_message>
EU industry + data improvements
from EU-BAT and US bandwidth study

Also moved things to an archive folder
</commit_message>
<xml_diff>
--- a/data/steel/bb_steel_factories.xlsx
+++ b/data/steel/bb_steel_factories.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29FD45C-7DF5-3A4E-A95C-2214DD170496}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="700" windowWidth="26520" windowHeight="17240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="705" windowWidth="26520" windowHeight="17235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bf-eaf chains" sheetId="9" r:id="rId1"/>
     <sheet name="bf-eaf connections" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>meta-process</t>
   </si>
@@ -101,15 +100,12 @@
   </si>
   <si>
     <t>bb_steel_bf-eaf</t>
-  </si>
-  <si>
-    <t>electricity__import</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -484,22 +480,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -516,7 +512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -530,7 +526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -550,21 +546,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" activeCellId="1" sqref="E2 E25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.875" customWidth="1"/>
+    <col min="6" max="6" width="14.875" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
@@ -573,7 +569,7 @@
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -611,7 +607,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -622,7 +618,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
@@ -637,24 +633,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" s="3"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="6"/>
       <c r="E9" s="2"/>
       <c r="F9" s="5"/>
@@ -662,7 +658,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="E10" s="7"/>
       <c r="F10" s="5"/>
@@ -670,7 +666,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="5"/>
@@ -678,7 +674,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -687,7 +683,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -696,7 +692,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -705,7 +701,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -714,7 +710,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -723,7 +719,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -733,7 +729,7 @@
       <c r="J17" s="2"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -742,7 +738,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>

</xml_diff>